<commit_message>
Perbaharuan File Nilai 1
</commit_message>
<xml_diff>
--- a/Olah Nilai/AI Task 4D Result/AI Task 5 - Neural Network (Jawaban).xlsx
+++ b/Olah Nilai/AI Task 4D Result/AI Task 5 - Neural Network (Jawaban).xlsx
@@ -1,12 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="600" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$G$30</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -295,25 +301,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -321,7 +330,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -337,45 +346,36 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -565,26 +565,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="12" width="18.88"/>
+    <col min="1" max="12" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,55 +610,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" s="3">
-        <v>45421.553408935186</v>
+        <v>45422.605948101853</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2">
-        <v>2.210631170089E12</v>
+        <v>2210631170014</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
-        <v>45421.84946203703</v>
+        <v>45422.623026134257</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2">
-        <v>2.210631170094E12</v>
+        <v>2210631170025</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3">
-        <v>45421.91751195602</v>
+        <v>45421.917511956017</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -667,225 +670,225 @@
         <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>2.210631170026E12</v>
+        <v>2210631170026</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
-        <v>45421.92648649306</v>
+        <v>45422.862582222224</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2">
-        <v>2.210631170079E12</v>
+        <v>2210631170027</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="G5" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3">
-        <v>45421.93613554398</v>
+        <v>45422.955261550931</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2210631170027</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
+        <v>45422.376543842591</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2210631170028</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3">
+        <v>45421.936135543983</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
-        <v>2.210631170029E12</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E8" s="2">
+        <v>2210631170029</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2">
-        <v>92.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3">
-        <v>45421.98605569445</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.210631170123E12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>45422.01965263889</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2.310631170162E12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="G8" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="3">
-        <v>45422.37654384259</v>
+        <v>45422.810302291662</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
-        <v>2.210631170028E12</v>
+        <v>2210631170030</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="3">
-        <v>45422.39839967593</v>
+        <v>45422.757616851857</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2">
-        <v>2.210631170118E12</v>
+        <v>2210631170031</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="5">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3">
-        <v>45422.60594810185</v>
+        <v>45422.852460173614</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2">
-        <v>2.210631170014E12</v>
+        <v>2210631170032</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>59</v>
+      </c>
+      <c r="G11" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="3">
-        <v>45422.62302613426</v>
+        <v>45422.982527881948</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2">
-        <v>2.210631170025E12</v>
+        <v>2210631170071</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="3">
-        <v>45422.75761685186</v>
+        <v>45423.012833449073</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2">
-        <v>2.210631170031E12</v>
+        <v>2210631170072</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="G13" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="3">
-        <v>45422.77705885417</v>
+        <v>45422.777058854168</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>44</v>
@@ -897,16 +900,16 @@
         <v>44</v>
       </c>
       <c r="E14" s="2">
-        <v>2.210631170073E12</v>
+        <v>2210631170073</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="G14" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="3">
         <v>45422.780382048615</v>
       </c>
@@ -920,248 +923,248 @@
         <v>47</v>
       </c>
       <c r="E15" s="2">
-        <v>2.210631170074E12</v>
+        <v>2210631170074</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="3">
-        <v>45422.81030229166</v>
+        <v>45422.832785324077</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E16" s="2">
-        <v>2.21063117003E12</v>
+        <v>2210631170075</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G16" s="2">
-        <v>85.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="3">
-        <v>45422.83278532408</v>
+        <v>45422.980148472227</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="E17" s="2">
-        <v>2.210631170075E12</v>
+        <v>2210631170076</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="G17" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="3">
-        <v>45422.85246017361</v>
+        <v>45422.881134895833</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E18" s="2">
-        <v>2.210631170032E12</v>
+        <v>2210631170077</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="6">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>65</v>
+      </c>
+      <c r="G18" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="3">
-        <v>45422.862582222224</v>
+        <v>45422.964081932871</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2">
-        <v>2.210631170027E12</v>
+        <v>2210631170078</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3">
-        <v>45422.88113489583</v>
+        <v>45421.926486493059</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E20" s="2">
-        <v>2.210631170077E12</v>
+        <v>2210631170079</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3">
-        <v>45422.88189945601</v>
+        <v>45421.553408935186</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2210631170089</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3">
+        <v>45421.849462037033</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2210631170094</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3">
+        <v>45422.881899456013</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="2">
-        <v>2.210631170117E12</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="E23" s="2">
+        <v>2210631170117</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="2">
-        <v>95.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3">
-        <v>45422.90092407407</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2.210631170149E12</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="2">
-        <v>88.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3">
-        <v>45422.92930166666</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="G23" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3">
+        <v>45422.398399675927</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="2">
-        <v>2.210631170118E12</v>
-      </c>
-      <c r="F23" s="4" t="s">
+      <c r="E24" s="2">
+        <v>2210631170118</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="3">
+        <v>45422.929301666663</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2210631170118</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3">
-        <v>45422.95526155093</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2.210631170027E12</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="3">
-        <v>45422.96408193287</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2.210631170078E12</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="G25" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="3">
-        <v>45422.96772881944</v>
+        <v>45422.967728819443</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>77</v>
@@ -1173,139 +1176,144 @@
         <v>77</v>
       </c>
       <c r="E26" s="2">
-        <v>2.210631170119E12</v>
+        <v>2210631170119</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G26" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="3">
-        <v>45422.98014847223</v>
+        <v>45423.000334629629</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2">
-        <v>2.210631170076E12</v>
+        <v>2210631170121</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G27" s="2">
-        <v>85.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="3">
-        <v>45422.98252788195</v>
+        <v>45421.986055694448</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2">
-        <v>2.210631170071E12</v>
+        <v>2210631170123</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G28" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="3">
-        <v>45423.00033462963</v>
+        <v>45422.900924074071</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2210631170149</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="2">
         <v>88</v>
       </c>
-      <c r="E29" s="2">
-        <v>2.210631170121E12</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="2">
-        <v>90.0</v>
-      </c>
-    </row>
-    <row r="30">
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="3">
-        <v>45423.01283344907</v>
+        <v>45422.01965263889</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="E30" s="2">
-        <v>2.210631170072E12</v>
+        <v>2310631170162</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="G30" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G30">
+    <sortState ref="A2:G30">
+      <sortCondition ref="B1:B30"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
-    <hyperlink r:id="rId7" ref="F8"/>
-    <hyperlink r:id="rId8" ref="F9"/>
-    <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId10" ref="F11"/>
-    <hyperlink r:id="rId11" ref="F12"/>
-    <hyperlink r:id="rId12" ref="F13"/>
-    <hyperlink r:id="rId13" ref="F14"/>
-    <hyperlink r:id="rId14" ref="F15"/>
-    <hyperlink r:id="rId15" ref="F16"/>
-    <hyperlink r:id="rId16" ref="F17"/>
-    <hyperlink r:id="rId17" ref="F18"/>
-    <hyperlink r:id="rId18" ref="F19"/>
-    <hyperlink r:id="rId19" ref="F20"/>
-    <hyperlink r:id="rId20" ref="F21"/>
-    <hyperlink r:id="rId21" ref="F22"/>
-    <hyperlink r:id="rId22" ref="F23"/>
-    <hyperlink r:id="rId23" ref="F24"/>
-    <hyperlink r:id="rId24" ref="F25"/>
-    <hyperlink r:id="rId25" ref="F26"/>
-    <hyperlink r:id="rId26" ref="F27"/>
-    <hyperlink r:id="rId27" ref="F28"/>
-    <hyperlink r:id="rId28" ref="F29"/>
-    <hyperlink r:id="rId29" ref="F30"/>
+    <hyperlink ref="F21" r:id="rId1"/>
+    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F20" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="F28" r:id="rId6"/>
+    <hyperlink ref="F30" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F24" r:id="rId9"/>
+    <hyperlink ref="F2" r:id="rId10"/>
+    <hyperlink ref="F3" r:id="rId11"/>
+    <hyperlink ref="F10" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F9" r:id="rId15"/>
+    <hyperlink ref="F16" r:id="rId16"/>
+    <hyperlink ref="F11" r:id="rId17"/>
+    <hyperlink ref="F5" r:id="rId18"/>
+    <hyperlink ref="F18" r:id="rId19"/>
+    <hyperlink ref="F23" r:id="rId20"/>
+    <hyperlink ref="F29" r:id="rId21"/>
+    <hyperlink ref="F25" r:id="rId22"/>
+    <hyperlink ref="F6" r:id="rId23"/>
+    <hyperlink ref="F19" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+    <hyperlink ref="F17" r:id="rId26"/>
+    <hyperlink ref="F12" r:id="rId27"/>
+    <hyperlink ref="F27" r:id="rId28"/>
+    <hyperlink ref="F13" r:id="rId29"/>
   </hyperlinks>
-  <drawing r:id="rId30"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>